<commit_message>
780 refresh larrabeiti table 1 with pathway descriptors
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -1,46 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C9F583-8493-7140-9EC7-86AA9D118F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361261B2-0872-6F45-959C-D0B5A6AFAAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="2" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="34560" windowHeight="20060" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Training_m54" sheetId="10" r:id="rId2"/>
+    <sheet name="Sheet4 (2)" sheetId="9" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet4!$A$21</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet4!$A$22</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Sheet4!$B$25:$E$25</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Sheet4!$A$21:$A$25</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Sheet4!$B$20</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Sheet4!$B$21:$B$25</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Sheet4!$C$20</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Sheet4!$C$21:$C$25</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">Sheet4!$D$20</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Sheet4!$D$21:$D$25</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">Sheet4!$E$20</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">Sheet4!$E$21:$E$25</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet4!$A$23</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet4!$A$24</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet4!$A$25</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet4!$B$20:$E$20</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet4!$B$21:$E$21</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Sheet4!$B$22:$E$22</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">Sheet4!$B$23:$E$23</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Sheet4!$B$24:$E$24</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,256 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="158">
-  <si>
-    <t>hsa-mir-1245b</t>
-  </si>
-  <si>
-    <t>hsa-mir-125b</t>
-  </si>
-  <si>
-    <t>hsa-mir-130a</t>
-  </si>
-  <si>
-    <t>hsa-mir-143</t>
-  </si>
-  <si>
-    <t>hsa-mir-144</t>
-  </si>
-  <si>
-    <t>hsa-mir-145</t>
-  </si>
-  <si>
-    <t>hsa-mir-146a</t>
-  </si>
-  <si>
-    <t>hsa-mir-146b</t>
-  </si>
-  <si>
-    <t>hsa-mir-155</t>
-  </si>
-  <si>
-    <t>hsa-mir-15a</t>
-  </si>
-  <si>
-    <t>hsa-mir-16-1</t>
-  </si>
-  <si>
-    <t>hsa-mir-17</t>
-  </si>
-  <si>
-    <t>hsa-mir-181a</t>
-  </si>
-  <si>
-    <t>hsa-mir-18a</t>
-  </si>
-  <si>
-    <t>hsa-mir-19a</t>
-  </si>
-  <si>
-    <t>hsa-mir-19b</t>
-  </si>
-  <si>
-    <t>hsa-mir-200c</t>
-  </si>
-  <si>
-    <t>hsa-mir-20a</t>
-  </si>
-  <si>
-    <t>hsa-mir-21</t>
-  </si>
-  <si>
-    <t>hsa-mir-210</t>
-  </si>
-  <si>
-    <t>hsa-mir-217</t>
-  </si>
-  <si>
-    <t>hsa-mir-221</t>
-  </si>
-  <si>
-    <t>hsa-mir-27b</t>
-  </si>
-  <si>
-    <t>hsa-mir-29c</t>
-  </si>
-  <si>
-    <t>hsa-mir-3156</t>
-  </si>
-  <si>
-    <t>hsa-mir-329</t>
-  </si>
-  <si>
-    <t>hsa-mir-34a</t>
-  </si>
-  <si>
-    <t>hsa-mir-3681</t>
-  </si>
-  <si>
-    <t>hsa-mir-378f</t>
-  </si>
-  <si>
-    <t>hsa-mir-379</t>
-  </si>
-  <si>
-    <t>hsa-mir-3922</t>
-  </si>
-  <si>
-    <t>hsa-mir-4263</t>
-  </si>
-  <si>
-    <t>hsa-mir-4510</t>
-  </si>
-  <si>
-    <t>hsa-mir-4511</t>
-  </si>
-  <si>
-    <t>hsa-mir-4516</t>
-  </si>
-  <si>
-    <t>hsa-mir-451b</t>
-  </si>
-  <si>
-    <t>hsa-mir-4647</t>
-  </si>
-  <si>
-    <t>hsa-mir-4721</t>
-  </si>
-  <si>
-    <t>hsa-mir-4727</t>
-  </si>
-  <si>
-    <t>hsa-mir-4793</t>
-  </si>
-  <si>
-    <t>hsa-mir-5010</t>
-  </si>
-  <si>
-    <t>hsa-mir-524</t>
-  </si>
-  <si>
-    <t>hsa-mir-585</t>
-  </si>
-  <si>
-    <t>hsa-mir-6133</t>
-  </si>
-  <si>
-    <t>hsa-mir-626</t>
-  </si>
-  <si>
-    <t>hsa-mir-6505</t>
-  </si>
-  <si>
-    <t>hsa-mir-6780a</t>
-  </si>
-  <si>
-    <t>hsa-mir-6827</t>
-  </si>
-  <si>
-    <t>hsa-mir-876</t>
-  </si>
-  <si>
-    <t>hsa-mir-92a</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>hsa-mir-1229</t>
-  </si>
-  <si>
-    <t>hsa-mir-1250</t>
-  </si>
-  <si>
-    <t>hsa-mir-129-1</t>
-  </si>
-  <si>
-    <t>hsa-mir-302c</t>
-  </si>
-  <si>
-    <t>hsa-mir-30b</t>
-  </si>
-  <si>
-    <t>hsa-mir-369</t>
-  </si>
-  <si>
-    <t>hsa-mir-371b</t>
-  </si>
-  <si>
-    <t>hsa-mir-378h</t>
-  </si>
-  <si>
-    <t>hsa-mir-4324</t>
-  </si>
-  <si>
-    <t>hsa-mir-4424</t>
-  </si>
-  <si>
-    <t>hsa-mir-449c</t>
-  </si>
-  <si>
-    <t>hsa-mir-4517</t>
-  </si>
-  <si>
-    <t>hsa-mir-4695</t>
-  </si>
-  <si>
-    <t>hsa-mir-4735</t>
-  </si>
-  <si>
-    <t>hsa-mir-4756</t>
-  </si>
-  <si>
-    <t>hsa-mir-4804</t>
-  </si>
-  <si>
-    <t>hsa-mir-5002</t>
-  </si>
-  <si>
-    <t>hsa-mir-5100</t>
-  </si>
-  <si>
-    <t>hsa-mir-551b</t>
-  </si>
-  <si>
-    <t>hsa-mir-5584</t>
-  </si>
-  <si>
-    <t>hsa-mir-577</t>
-  </si>
-  <si>
-    <t>hsa-mir-6086</t>
-  </si>
-  <si>
-    <t>hsa-mir-6510</t>
-  </si>
-  <si>
-    <t>hsa-mir-6782</t>
-  </si>
-  <si>
-    <t>hsa-mir-6794</t>
-  </si>
-  <si>
-    <t>hsa-mir-7855</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>accuracy</t>
   </si>
@@ -332,165 +59,6 @@
   </si>
   <si>
     <t>MLP</t>
-  </si>
-  <si>
-    <t>hsa-let-7d</t>
-  </si>
-  <si>
-    <t>hsa-let-7e</t>
-  </si>
-  <si>
-    <t>hsa-let-7g</t>
-  </si>
-  <si>
-    <t>hsa-let-7i</t>
-  </si>
-  <si>
-    <t>hsa-mir-100</t>
-  </si>
-  <si>
-    <t>hsa-mir-101</t>
-  </si>
-  <si>
-    <t>hsa-mir-103a</t>
-  </si>
-  <si>
-    <t>hsa-mir-105</t>
-  </si>
-  <si>
-    <t>hsa-mir-106a</t>
-  </si>
-  <si>
-    <t>hsa-mir-106b</t>
-  </si>
-  <si>
-    <t>hsa-mir-107</t>
-  </si>
-  <si>
-    <t>hsa-mir-10b</t>
-  </si>
-  <si>
-    <t>hsa-mir-126</t>
-  </si>
-  <si>
-    <t>hsa-mir-128</t>
-  </si>
-  <si>
-    <t>hsa-mir-130b</t>
-  </si>
-  <si>
-    <t>hsa-mir-142</t>
-  </si>
-  <si>
-    <t>hsa-mir-150</t>
-  </si>
-  <si>
-    <t>hsa-mir-15b</t>
-  </si>
-  <si>
-    <t>hsa-mir-16</t>
-  </si>
-  <si>
-    <t>hsa-mir-181b</t>
-  </si>
-  <si>
-    <t>hsa-mir-182</t>
-  </si>
-  <si>
-    <t>hsa-mir-183</t>
-  </si>
-  <si>
-    <t>hsa-mir-18b</t>
-  </si>
-  <si>
-    <t>hsa-mir-196b</t>
-  </si>
-  <si>
-    <t>hsa-mir-199a</t>
-  </si>
-  <si>
-    <t>hsa-mir-199b</t>
-  </si>
-  <si>
-    <t>hsa-mir-206</t>
-  </si>
-  <si>
-    <t>hsa-mir-22</t>
-  </si>
-  <si>
-    <t>hsa-mir-222</t>
-  </si>
-  <si>
-    <t>hsa-mir-24</t>
-  </si>
-  <si>
-    <t>hsa-mir-25</t>
-  </si>
-  <si>
-    <t>hsa-mir-30a</t>
-  </si>
-  <si>
-    <t>hsa-mir-30d</t>
-  </si>
-  <si>
-    <t>hsa-mir-320a</t>
-  </si>
-  <si>
-    <t>hsa-mir-328</t>
-  </si>
-  <si>
-    <t>hsa-mir-33a</t>
-  </si>
-  <si>
-    <t>hsa-mir-342</t>
-  </si>
-  <si>
-    <t>hsa-mir-34b</t>
-  </si>
-  <si>
-    <t>hsa-mir-362</t>
-  </si>
-  <si>
-    <t>hsa-mir-365a</t>
-  </si>
-  <si>
-    <t>hsa-mir-374a</t>
-  </si>
-  <si>
-    <t>hsa-mir-425</t>
-  </si>
-  <si>
-    <t>hsa-mir-485</t>
-  </si>
-  <si>
-    <t>hsa-mir-487b</t>
-  </si>
-  <si>
-    <t>hsa-mir-518a</t>
-  </si>
-  <si>
-    <t>hsa-mir-582</t>
-  </si>
-  <si>
-    <t>hsa-mir-636</t>
-  </si>
-  <si>
-    <t>hsa-mir-660</t>
-  </si>
-  <si>
-    <t>hsa-mir-7</t>
-  </si>
-  <si>
-    <t>hsa-mir-9</t>
-  </si>
-  <si>
-    <t>hsa-mir-92b</t>
-  </si>
-  <si>
-    <t>hsa-mir-93</t>
-  </si>
-  <si>
-    <t>hsa-mir-98</t>
   </si>
   <si>
     <t>IBk</t>
@@ -536,6 +104,18 @@
   </si>
   <si>
     <t>Independent Dataset 3 [12]</t>
+  </si>
+  <si>
+    <t>ZeroR (InfoGain 0.01)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 1</t>
+  </si>
+  <si>
+    <t>Independent Dataset 2</t>
+  </si>
+  <si>
+    <t>Independent Dataset 3</t>
   </si>
 </sst>
 </file>
@@ -2087,6 +1667,1072 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6BF3-C847-B936-7B74A9D7FE5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of the Training</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Dataset (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Training_m54!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Training_m54!$A$21:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>RF (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LMT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLP (CfsSubsetEval)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SMO (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ZeroR (InfoGain 0.01)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Training_m54!$B$21:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.75925900000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76851899999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.796296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80555600000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76851899999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46296300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DF5-7D40-8F48-84BDAE5AFAF2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>RF (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LMT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLP (CfsSubsetEval)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SMO (InfoGain 0.01)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet4 (2)'!$B$21:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.77777799999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77780000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72222200000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83333299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88888900000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D941-1945-AA78-25BB9FB74980}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>RF (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LMT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLP (CfsSubsetEval)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SMO (InfoGain 0.01)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet4 (2)'!$C$21:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D941-1945-AA78-25BB9FB74980}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>RF (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LMT (InfoGain 0.01)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLP (CfsSubsetEval)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SMO (InfoGain 0.01)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet4 (2)'!$D$21:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.47058800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41176499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58823499999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52941199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.764706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D941-1945-AA78-25BB9FB74980}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2406,6 +3052,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -3480,6 +4206,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4095,52 +5827,90 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{877AD36B-ACC7-5849-818F-2BBA82C1FD57}" name="Table3" displayName="Table3" ref="A1:G51" totalsRowShown="0">
-  <autoFilter ref="A1:G51" xr:uid="{877AD36B-ACC7-5849-818F-2BBA82C1FD57}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D63CDC7E-B414-694D-9932-59B1B84C06C9}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{2B1B96DC-A7B3-454C-BE9E-234CD6D26582}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{8D69D395-DF51-2D40-88E1-CC87FEDB19CE}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{C317D908-ACDB-A84B-8BF2-96FF3F6FCF7F}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{5998FB64-D9C8-954E-B479-5BD333D8A803}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{5FF48ACD-4FE4-E749-B57B-627A9357863B}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{CC045930-909E-C749-B18F-3D53F5353C48}" name="Column7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2063750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>624416</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39A4F933-958C-2946-A022-100D5EF24542}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{118D5E16-E763-454A-B606-C3FAE068DD63}" name="Table7" displayName="Table7" ref="A1:G41" totalsRowShown="0">
-  <autoFilter ref="A1:G41" xr:uid="{118D5E16-E763-454A-B606-C3FAE068DD63}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{977600CF-F0AD-C44C-8DAD-FB8692D39884}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{84059611-D4B2-024B-8B3A-ECDD61706EF5}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{B87F49A1-2F8F-0C41-B8F0-795FA6082795}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{341491B9-BF7B-AA47-A183-B83BC102CAD3}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{4BFA90CC-106F-5A42-BA89-CC2AB229E71C}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{B24BB0CB-9B4B-C340-9ACF-6671A1B2F6B5}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{A2DC6E57-E3A2-C745-BBEA-B1CA452757F0}" name="Column7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{67BA1DB3-E2C3-9A44-BCAE-E815821DB0F7}" name="Table4" displayName="Table4" ref="A1:G30" totalsRowShown="0">
-  <autoFilter ref="A1:G30" xr:uid="{67BA1DB3-E2C3-9A44-BCAE-E815821DB0F7}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4B854406-9A73-6D4D-A4F8-64F2DE6F9E96}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{4369C337-C29F-9649-9E5B-98AB821A76AA}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{7DCA4678-0FB6-7346-A6B6-3314E9D11FDF}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{DDBDB245-098C-6D40-BEDD-08F01F013165}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{CC989893-8536-EC4A-87DD-243A0FFC0D07}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{FA1A0030-B5F6-0148-A921-D62C310DB295}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{947E670E-7FCD-8141-8A2A-312C7E3FDD9E}" name="Column7"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>110064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>179915</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D96BA09-4AA2-4E4B-928A-A22B569BD798}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4439,556 +6209,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCFBA2A-DFE3-7F43-81E0-A9138AC9A703}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G51"/>
-  <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="89" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69457ADA-6A95-F945-9737-D71FDB676797}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC799B3-39DE-6347-8E4B-64801D276C28}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -5003,15 +6227,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>73.529399999999995</v>
@@ -5019,7 +6243,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>85.2941</v>
@@ -5027,7 +6251,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>70.588200000000001</v>
@@ -5035,7 +6259,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>73.529399999999995</v>
@@ -5043,7 +6267,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>73.529399999999995</v>
@@ -5051,21 +6275,21 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>0.75925900000000002</v>
@@ -5080,7 +6304,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>0.75</v>
@@ -5095,7 +6319,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>0.74074099999999998</v>
@@ -5110,7 +6334,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>0.75</v>
@@ -5125,7 +6349,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>0.75</v>
@@ -5140,7 +6364,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>0.99074099999999998</v>
@@ -5167,24 +6391,24 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
         <v>0.72222200000000003</v>
@@ -5201,7 +6425,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>0.74074099999999998</v>
@@ -5218,7 +6442,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
         <v>0.75</v>
@@ -5235,7 +6459,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
         <v>0.75</v>
@@ -5252,7 +6476,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <v>0.75925900000000002</v>
@@ -5274,573 +6498,282 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF53B68-F6B9-E147-B52A-5FD71DCAAA53}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G30"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9430B7F4-BBA4-D54C-9C5B-54149D51A68E}">
+  <dimension ref="A9:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>29</v>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>65</v>
-      </c>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.75925900000000002</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.76851899999999995</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.796296</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.80555600000000005</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>69</v>
-      </c>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.76851899999999995</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>82</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.46296300000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B07664C-6D19-4E40-B124-26022900FB4F}">
-  <dimension ref="A1:A72"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C1234B-43CE-FD4F-989C-2D3733D0ABDF}">
+  <dimension ref="A9:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>90</v>
-      </c>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>96</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.77777799999999997</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.47058800000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>98</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.41176499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>99</v>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.72222200000000003</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.58823499999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>100</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.52941199999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>142</v>
+      <c r="B25" s="1">
+        <v>0.88888900000000004</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.764706</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
860 Create a new testing set based on Beheshti's paper
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361261B2-0872-6F45-959C-D0B5A6AFAAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CD63BC-6AFC-9647-B924-E8EAE4C27ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="34560" windowHeight="20060" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="4" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
     <sheet name="Training_m54" sheetId="10" r:id="rId2"/>
-    <sheet name="Sheet4 (2)" sheetId="9" r:id="rId3"/>
+    <sheet name="Testing Sets" sheetId="9" r:id="rId3"/>
+    <sheet name="Training_m54 (2)" sheetId="11" r:id="rId4"/>
+    <sheet name="Testing Sets (2)" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>accuracy</t>
   </si>
@@ -117,6 +119,15 @@
   <si>
     <t>Independent Dataset 3</t>
   </si>
+  <si>
+    <t>Attribut Selection: weka.filters.supervised.attribute.AttributeSelection -E "weka.attributeSelection.CfsSubsetEval -P 1 -E 1" -S "weka.attributeSelection.BestFirst -D 1 -N 5"</t>
+  </si>
+  <si>
+    <t>ZeroR</t>
+  </si>
+  <si>
+    <t>BayesNet</t>
+  </si>
 </sst>
 </file>
 
@@ -151,10 +162,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2339,7 +2353,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$B$20</c:f>
+              <c:f>'Testing Sets'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2417,7 +2431,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:f>'Testing Sets'!$A$21:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2440,7 +2454,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet4 (2)'!$B$21:$B$25</c:f>
+              <c:f>'Testing Sets'!$B$21:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2473,7 +2487,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$C$20</c:f>
+              <c:f>'Testing Sets'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2551,7 +2565,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:f>'Testing Sets'!$A$21:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2574,7 +2588,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet4 (2)'!$C$21:$C$25</c:f>
+              <c:f>'Testing Sets'!$C$21:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2607,7 +2621,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$D$20</c:f>
+              <c:f>'Testing Sets'!$D$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2685,7 +2699,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet4 (2)'!$A$21:$A$25</c:f>
+              <c:f>'Testing Sets'!$A$21:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2708,7 +2722,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet4 (2)'!$D$21:$D$25</c:f>
+              <c:f>'Testing Sets'!$D$21:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2733,6 +2747,1048 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D941-1945-AA78-25BB9FB74980}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of the Training</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Dataset (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Training_m54 (2)'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Training_m54 (2)'!$A$21:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>BayesNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RF</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ZeroR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Training_m54 (2)'!$B$21:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.91666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93518500000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94444399999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86111099999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46296300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-53B0-1F40-A9CB-F03BCB983AF5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>BayesNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Sets (2)'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.88888900000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88888900000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88888900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88888900000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6EBA-704D-89D9-5307AA4AEC59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>BayesNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Sets (2)'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6EBA-704D-89D9-5307AA4AEC59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Sets (2)'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>BayesNet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Sets (2)'!$D$21:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.64705900000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70588200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64705900000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58823499999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6EBA-704D-89D9-5307AA4AEC59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3132,6 +4188,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -5212,6 +6348,1012 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5913,6 +8055,92 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2063750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>74084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>624416</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBEB5B0-71EF-8E43-9CB7-BA9E032F40D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>110064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>179915</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3125CA67-A67C-A04A-AB01-18114203B841}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6212,7 +8440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC799B3-39DE-6347-8E4B-64801D276C28}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="C13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -6776,4 +9004,264 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAD6438-12C1-8247-95B5-C0F78C60B61A}">
+  <dimension ref="A9:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.93518500000000004</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.94444399999999995</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.86111099999999996</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.46296300000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09694F6F-64A6-AD4F-BABD-AC8EE9073979}">
+  <dimension ref="A9:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.88888900000000004</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.64705900000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.88888900000000004</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.70588200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.88888900000000004</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.64705900000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.88888900000000004</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.58823499999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
880 regenerate training and testing sets
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CD63BC-6AFC-9647-B924-E8EAE4C27ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A91EDDD-584C-D94C-9F90-727DDDC3ABBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="4" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>accuracy</t>
   </si>
@@ -126,7 +126,13 @@
     <t>ZeroR</t>
   </si>
   <si>
-    <t>BayesNet</t>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Bayes Network</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
   </si>
 </sst>
 </file>
@@ -3114,16 +3120,16 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>BayesNet</c:v>
+                  <c:v>Bayes Network</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Logistic</c:v>
+                  <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>MLP</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RF</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>ZeroR</c:v>
@@ -3144,7 +3150,7 @@
                   <c:v>0.93518500000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94444399999999995</c:v>
+                  <c:v>0.87963000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.86111099999999996</c:v>
@@ -3495,16 +3501,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>BayesNet</c:v>
+                  <c:v>Bayes Network</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Logistic</c:v>
+                  <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>MLP</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RF</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3623,16 +3629,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>BayesNet</c:v>
+                  <c:v>Bayes Network</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Logistic</c:v>
+                  <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>MLP</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RF</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3644,7 +3650,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.85</c:v>
@@ -3751,16 +3757,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>BayesNet</c:v>
+                  <c:v>Bayes Network</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Logistic</c:v>
+                  <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>MLP</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RF</c:v>
+                  <c:v>Random Forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3772,16 +3778,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.64705900000000005</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70588200000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64705900000000005</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58823499999999995</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3860,6 +3866,7 @@
         <c:axId val="1833862175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -9011,7 +9018,7 @@
   <dimension ref="A9:E27"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B25"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9081,7 +9088,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1">
         <v>0.91666700000000001</v>
@@ -9092,7 +9099,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1">
         <v>0.93518500000000004</v>
@@ -9106,7 +9113,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="1">
-        <v>0.94444399999999995</v>
+        <v>0.87963000000000002</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -9114,7 +9121,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>0.86111099999999996</v>
@@ -9148,7 +9155,7 @@
   <dimension ref="A9:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9205,21 +9212,21 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1">
         <v>0.88888900000000004</v>
       </c>
       <c r="C21" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D21" s="1">
-        <v>0.64705900000000005</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1">
         <v>0.88888900000000004</v>
@@ -9228,7 +9235,7 @@
         <v>0.85</v>
       </c>
       <c r="D22" s="1">
-        <v>0.70588200000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9242,12 +9249,12 @@
         <v>0.9</v>
       </c>
       <c r="D23" s="1">
-        <v>0.64705900000000005</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>0.88888900000000004</v>
@@ -9256,7 +9263,7 @@
         <v>0.85</v>
       </c>
       <c r="D24" s="1">
-        <v>0.58823499999999995</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
910 add mir-189 and mir-768 in Lawrie's table 1
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A91EDDD-584C-D94C-9F90-727DDDC3ABBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB5F32-B862-BA44-961A-75DB4E3FA7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="4" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="5" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Testing Sets" sheetId="9" r:id="rId3"/>
     <sheet name="Training_m54 (2)" sheetId="11" r:id="rId4"/>
     <sheet name="Testing Sets (2)" sheetId="12" r:id="rId5"/>
+    <sheet name="Testing Sets (3)" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>accuracy</t>
   </si>
@@ -133,6 +134,12 @@
   </si>
   <si>
     <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Independent Dataset 1 (full)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 1 (clean)</t>
   </si>
 </sst>
 </file>
@@ -3795,6 +3802,540 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6EBA-704D-89D9-5307AA4AEC59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Sets (3)'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 1 (full)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Sets (3)'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Sets (3)'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42DB-7740-B591-DD4473F0A1D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Sets (3)'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 1 (clean)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Sets (3)'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Sets (3)'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-42DB-7740-B591-DD4473F0A1D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4275,6 +4816,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -7361,6 +7942,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8148,6 +9232,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>191708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>61987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AEB90AA-0E8B-F942-8121-ED0E560ED4DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9154,7 +10281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09694F6F-64A6-AD4F-BABD-AC8EE9073979}">
   <dimension ref="A9:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -9271,4 +10398,105 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F4405E-39B3-F446-83B1-82BFFF4C949B}">
+  <dimension ref="A9:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
920 generate clean testing sets (no overlaping miRNAs)
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB5F32-B862-BA44-961A-75DB4E3FA7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA287E0-9315-A74C-B1BC-F5EA3500B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="5" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="6" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="Testing Sets" sheetId="9" r:id="rId3"/>
     <sheet name="Training_m54 (2)" sheetId="11" r:id="rId4"/>
     <sheet name="Testing Sets (2)" sheetId="12" r:id="rId5"/>
-    <sheet name="Testing Sets (3)" sheetId="13" r:id="rId6"/>
+    <sheet name="Testing Set #1" sheetId="13" r:id="rId6"/>
+    <sheet name="Testing Set #2" sheetId="14" r:id="rId7"/>
+    <sheet name="Testing Set #3" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>accuracy</t>
   </si>
@@ -140,6 +142,18 @@
   </si>
   <si>
     <t>Independent Dataset 1 (clean)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 2 (full)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 2 (clean)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 3 (full)</t>
+  </si>
+  <si>
+    <t>Independent Dataset 3 (clean)</t>
   </si>
 </sst>
 </file>
@@ -530,6 +544,522 @@
         <a:schemeClr val="dk1">
           <a:lumMod val="25000"/>
           <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set #3'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 3 (full)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set #3'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set #3'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-22CC-E940-8853-C116E6CAD813}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set #3'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 3 (clean)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set #3'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set #3'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-22CC-E940-8853-C116E6CAD813}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -4088,7 +4618,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Sets (3)'!$B$20</c:f>
+              <c:f>'Testing Set #1'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4166,7 +4696,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Sets (3)'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set #1'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -4186,21 +4716,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Sets (3)'!$B$21:$B$24</c:f>
+              <c:f>'Testing Set #1'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4216,7 +4737,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Sets (3)'!$C$20</c:f>
+              <c:f>'Testing Set #1'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4294,7 +4815,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Sets (3)'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set #1'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -4314,21 +4835,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Sets (3)'!$C$21:$C$24</c:f>
+              <c:f>'Testing Set #1'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85</c:v>
+                  <c:v>0.42857099999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4536,7 +5048,563 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set #2'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 2 (full)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set #2'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set #2'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CEE-F34A-8CFB-A6680E612DE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set #2'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent Dataset 2 (clean)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set #2'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set #2'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0CEE-F34A-8CFB-A6680E612DE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4856,6 +5924,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -5426,7 +6534,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5929,7 +7037,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6432,7 +7540,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6935,7 +8043,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7438,7 +8546,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7941,7 +9049,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8444,7 +9552,1013 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9275,6 +11389,92 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>191708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>61987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD53BE1-BBB1-5040-B4AA-18A597A7CDB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>191708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>61987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C40CF3-B0C8-E74C-9251-ED610D368A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10404,8 +12604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F4405E-39B3-F446-83B1-82BFFF4C949B}">
   <dimension ref="A9:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10458,41 +12658,207 @@
         <v>0.8</v>
       </c>
       <c r="C21" s="1">
-        <v>0.85</v>
+        <v>0.42857099999999998</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.85</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.9</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F03E7BA-9F7D-A740-A4F1-CA14538681F6}">
+  <dimension ref="A9:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
         <v>0.85</v>
       </c>
-      <c r="C24" s="1">
-        <v>0.85</v>
-      </c>
+      <c r="C21" s="1">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFA8ED1-E781-414D-8101-89DE2827F8EE}">
+  <dimension ref="A9:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
950 Generate pathway attributes for testing set Sun
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA287E0-9315-A74C-B1BC-F5EA3500B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE3FA8-7B5A-D045-B2D5-5198C63339F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="6" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="8" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Testing Sets" sheetId="9" r:id="rId3"/>
     <sheet name="Training_m54 (2)" sheetId="11" r:id="rId4"/>
     <sheet name="Testing Sets (2)" sheetId="12" r:id="rId5"/>
-    <sheet name="Testing Set #1" sheetId="13" r:id="rId6"/>
-    <sheet name="Testing Set #2" sheetId="14" r:id="rId7"/>
-    <sheet name="Testing Set #3" sheetId="15" r:id="rId8"/>
+    <sheet name="Testing Set Lawrie" sheetId="14" r:id="rId6"/>
+    <sheet name="Testing Set Behe" sheetId="15" r:id="rId7"/>
+    <sheet name="Testing Set Sun" sheetId="13" r:id="rId8"/>
+    <sheet name="Testing Set bou" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>accuracy</t>
   </si>
@@ -138,22 +139,19 @@
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Independent Dataset 1 (full)</t>
+    <t>Clean set of miRNAs</t>
   </si>
   <si>
-    <t>Independent Dataset 1 (clean)</t>
+    <t>Full set of miRNAs (54.55% overlapping)</t>
   </si>
   <si>
-    <t>Independent Dataset 2 (full)</t>
+    <t>Full set of miRNAs (55.56% overlapping)</t>
   </si>
   <si>
-    <t>Independent Dataset 2 (clean)</t>
+    <t>Full set of miRNAs (25.00% overlapping)</t>
   </si>
   <si>
-    <t>Independent Dataset 3 (full)</t>
-  </si>
-  <si>
-    <t>Independent Dataset 3 (clean)</t>
+    <t>Full set of miRNAs (57.14%% overlapping)</t>
   </si>
 </sst>
 </file>
@@ -607,7 +605,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+              <a:t> Data Set #1 (with Cross-validation 10-fold)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -654,11 +652,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #3'!$B$20</c:f>
+              <c:f>'Testing Set Sun'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 3 (full)</c:v>
+                  <c:v>Full set of miRNAs (25.00% overlapping)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -732,7 +730,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #3'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Sun'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -752,19 +750,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #3'!$B$21:$B$24</c:f>
+              <c:f>'Testing Set Sun'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-22CC-E940-8853-C116E6CAD813}"/>
+              <c16:uniqueId val="{00000000-42DB-7740-B591-DD4473F0A1D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -773,11 +780,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #3'!$C$20</c:f>
+              <c:f>'Testing Set Sun'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 3 (clean)</c:v>
+                  <c:v>Clean set of miRNAs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -851,7 +858,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #3'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Sun'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -871,19 +878,538 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #3'!$C$21:$C$24</c:f>
+              <c:f>'Testing Set Sun'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.83333299999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66666700000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83333299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-22CC-E940-8853-C116E6CAD813}"/>
+              <c16:uniqueId val="{00000001-42DB-7740-B591-DD4473F0A1D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1833715167"/>
+        <c:axId val="1833862175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1833715167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833862175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833862175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833715167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classifier Accuracy of Independent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Data Set #1 (with Cross-validation 10-fold)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set bou'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Full set of miRNAs (57.14%% overlapping)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set bou'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set bou'!$B$21:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5676-F248-83EE-64161AC86B6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Testing Set bou'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Clean set of miRNAs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Testing Set bou'!$A$21:$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Bayes Network</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Testing Set bou'!$C$21:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5676-F248-83EE-64161AC86B6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4618,11 +5144,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #1'!$B$20</c:f>
+              <c:f>'Testing Set Lawrie'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 1 (full)</c:v>
+                  <c:v>Full set of miRNAs (54.55% overlapping)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4696,7 +5222,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #1'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Lawrie'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -4716,19 +5242,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #1'!$B$21:$B$24</c:f>
+              <c:f>'Testing Set Lawrie'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.81818199999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81818199999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86363599999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81818199999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-42DB-7740-B591-DD4473F0A1D1}"/>
+              <c16:uniqueId val="{00000000-0CEE-F34A-8CFB-A6680E612DE8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4737,11 +5272,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #1'!$C$20</c:f>
+              <c:f>'Testing Set Lawrie'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 1 (clean)</c:v>
+                  <c:v>Clean set of miRNAs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4815,7 +5350,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #1'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Lawrie'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -4835,19 +5370,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #1'!$C$21:$C$24</c:f>
+              <c:f>'Testing Set Lawrie'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.42857099999999998</c:v>
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-42DB-7740-B591-DD4473F0A1D1}"/>
+              <c16:uniqueId val="{00000001-0CEE-F34A-8CFB-A6680E612DE8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5082,12 +5626,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Classifier Accuracy of Independent</a:t>
+              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Classifier Accuracy of Independent Data Set #3 </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+              <a:t>(with Cross-validation 10-fold)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -5134,11 +5685,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #2'!$B$20</c:f>
+              <c:f>'Testing Set Behe'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 2 (full)</c:v>
+                  <c:v>Full set of miRNAs (55.56% overlapping)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5212,7 +5763,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #2'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Behe'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5232,19 +5783,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #2'!$B$21:$B$24</c:f>
+              <c:f>'Testing Set Behe'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0CEE-F34A-8CFB-A6680E612DE8}"/>
+              <c16:uniqueId val="{00000000-22CC-E940-8853-C116E6CAD813}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5253,11 +5813,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set #2'!$C$20</c:f>
+              <c:f>'Testing Set Behe'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent Dataset 2 (clean)</c:v>
+                  <c:v>Clean set of miRNAs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5331,7 +5891,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set #2'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Behe'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5351,19 +5911,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set #2'!$C$21:$C$24</c:f>
+              <c:f>'Testing Set Behe'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0CEE-F34A-8CFB-A6680E612DE8}"/>
+              <c16:uniqueId val="{00000001-22CC-E940-8853-C116E6CAD813}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5605,6 +6174,46 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7037,6 +7646,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -11366,7 +12478,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AEB90AA-0E8B-F942-8121-ED0E560ED4DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD53BE1-BBB1-5040-B4AA-18A597A7CDB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11409,7 +12521,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD53BE1-BBB1-5040-B4AA-18A597A7CDB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C40CF3-B0C8-E74C-9251-ED610D368A8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11452,7 +12564,50 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C40CF3-B0C8-E74C-9251-ED610D368A8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AEB90AA-0E8B-F942-8121-ED0E560ED4DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>191708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>61987</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C14CC64D-A196-434D-8B80-12CBE42EB188}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12601,17 +13756,117 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F4405E-39B3-F446-83B1-82BFFF4C949B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F03E7BA-9F7D-A740-A4F1-CA14538681F6}">
   <dimension ref="A9:C24"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="3" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.81818199999999996</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.81818199999999996</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.86363599999999996</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.81818199999999996</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFA8ED1-E781-414D-8101-89DE2827F8EE}">
+  <dimension ref="A9:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12644,10 +13899,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -12655,32 +13910,44 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>0.42857099999999998</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12689,18 +13956,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F03E7BA-9F7D-A740-A4F1-CA14538681F6}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F4405E-39B3-F446-83B1-82BFFF4C949B}">
   <dimension ref="A9:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C24"/>
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12733,10 +14000,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -12744,32 +14011,44 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
       <c r="C21" s="1">
-        <v>0.625</v>
+        <v>0.83333299999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.66666700000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.66666700000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.83333299999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12778,18 +14057,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFA8ED1-E781-414D-8101-89DE2827F8EE}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE18E5D5-E200-E24C-B2C7-C5CB3599CC05}">
   <dimension ref="A9:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12825,19 +14104,15 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">

</xml_diff>

<commit_message>
970 Update Kegg diagram because its coloring format changed
</commit_message>
<xml_diff>
--- a/resources/results/classifier_comparison.xlsx
+++ b/resources/results/classifier_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE3FA8-7B5A-D045-B2D5-5198C63339F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5976437A-301B-904D-9AFC-75A6A05E1836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="8" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
+    <workbookView xWindow="-68800" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="3" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Testing Sets" sheetId="9" r:id="rId3"/>
     <sheet name="Training_m54 (2)" sheetId="11" r:id="rId4"/>
     <sheet name="Testing Sets (2)" sheetId="12" r:id="rId5"/>
-    <sheet name="Testing Set Lawrie" sheetId="14" r:id="rId6"/>
+    <sheet name="Testing Set Lawrie 2" sheetId="14" r:id="rId6"/>
     <sheet name="Testing Set Behe" sheetId="15" r:id="rId7"/>
     <sheet name="Testing Set Sun" sheetId="13" r:id="rId8"/>
     <sheet name="Testing Set bou" sheetId="16" r:id="rId9"/>
@@ -605,7 +605,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Data Set #1 (with Cross-validation 10-fold)</a:t>
+              <a:t> Data Set #3 (with Cross-validation 10-fold)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -5097,7 +5097,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Datasets (with Cross-validation 10-fold)</a:t>
+              <a:t> Dataset #1 (with Cross-validation 10-fold)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -5144,7 +5144,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set Lawrie'!$B$20</c:f>
+              <c:f>'Testing Set Lawrie 2'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5222,7 +5222,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set Lawrie'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Lawrie 2'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5242,7 +5242,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set Lawrie'!$B$21:$B$24</c:f>
+              <c:f>'Testing Set Lawrie 2'!$B$21:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5272,7 +5272,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Testing Set Lawrie'!$C$20</c:f>
+              <c:f>'Testing Set Lawrie 2'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5350,7 +5350,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Testing Set Lawrie'!$A$21:$A$24</c:f>
+              <c:f>'Testing Set Lawrie 2'!$A$21:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5370,7 +5370,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Testing Set Lawrie'!$C$21:$C$24</c:f>
+              <c:f>'Testing Set Lawrie 2'!$C$21:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5634,7 +5634,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Classifier Accuracy of Independent Data Set #3 </a:t>
+              <a:t>Classifier Accuracy of Independent Data Set #2 </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -13499,8 +13499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAD6438-12C1-8247-95B5-C0F78C60B61A}">
   <dimension ref="A9:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13760,7 +13760,7 @@
   <dimension ref="A9:C24"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14061,7 +14061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE18E5D5-E200-E24C-B2C7-C5CB3599CC05}">
   <dimension ref="A9:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>